<commit_message>
added kwh and engine types for more vessels
</commit_message>
<xml_diff>
--- a/Legacy data vessels.xlsx
+++ b/Legacy data vessels.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersEmilBusk\Desktop\Feedback report generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid.sharepoint.com/sites/MarineFluidTechnologyAS/Shared Documents/Projects/16. Feedback report to vessels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B07B958-9481-4337-BE77-39E9672A75B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{779D105B-5A6D-46FA-9EED-1DAB4054135F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEE69B7E-2F51-44BB-81C6-E6F8432A1C35}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="51420" windowHeight="13900" xr2:uid="{9994A8F6-3190-471E-B791-9B9DB550B49C}"/>
+    <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{9994A8F6-3190-471E-B791-9B9DB550B49C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,36 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F1E24293-0A3D-45D8-A7CD-AD75AE91C28D}</author>
+    <author>tc={6049E165-AEC7-4645-843F-7793999AB662}</author>
+  </authors>
+  <commentList>
+    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{F1E24293-0A3D-45D8-A7CD-AD75AE91C28D}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Hvorfor er denne I vores ark?
+</t>
+      </text>
+    </comment>
+    <comment ref="C112" authorId="1" shapeId="0" xr:uid="{6049E165-AEC7-4645-843F-7793999AB662}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Hvorfor er denne I vores ark?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="169">
   <si>
     <t>Adriatic Gas</t>
   </si>
@@ -528,16 +557,37 @@
   </si>
   <si>
     <t>fil_pur</t>
+  </si>
+  <si>
+    <t>6S60ME-C8</t>
+  </si>
+  <si>
+    <t>6S60ME-C9</t>
+  </si>
+  <si>
+    <t>6S50ME-B8</t>
+  </si>
+  <si>
+    <t>5RT-flex58T</t>
+  </si>
+  <si>
+    <t>5S46MC-C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -563,13 +613,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -583,7 +711,25 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Andreas Johansen" id="{35137BE2-117A-4679-BEED-025B241F47D5}" userId="S::andreas.johansen@marinefluid.dk::98c433f8-bfa1-410d-888b-0a36d16529be" providerId="AD"/>
+</personList>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6D1D042-62DD-4433-A9B7-CB1F28CECDBA}" name="Table1" displayName="Table1" ref="B2:H112" totalsRowShown="0">
+  <autoFilter ref="B2:H112" xr:uid="{E6D1D042-62DD-4433-A9B7-CB1F28CECDBA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F9278369-CA4C-4372-8BC1-3B75D5BFF97C}" name="imo_no" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{6533DEEE-46FF-472D-82C5-AABE46D63219}" name="customer" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A25C2A48-2EF6-4925-A55D-7B137A95B51E}" name="vessel_name"/>
+    <tableColumn id="3" xr3:uid="{D5F0F564-D630-4E12-B27E-7CAF9622FBD6}" name="en_manu" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{BD32E7A6-11C2-442B-8395-0ACA51659E54}" name="en_mod" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E6BD8EF1-3AFE-4FA0-A853-0776C1E55ADE}" name="mcr_out" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{D575CC75-08E1-4BE0-AA3A-B607E8D805EB}" name="fil_pur"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -901,1843 +1047,2029 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C41" dT="2025-03-20T10:29:21.52" personId="{35137BE2-117A-4679-BEED-025B241F47D5}" id="{F1E24293-0A3D-45D8-A7CD-AD75AE91C28D}">
+    <text xml:space="preserve">Hvorfor er denne I vores ark?
+</text>
+  </threadedComment>
+  <threadedComment ref="C112" dT="2025-03-20T10:29:38.02" personId="{35137BE2-117A-4679-BEED-025B241F47D5}" id="{6049E165-AEC7-4645-843F-7793999AB662}">
+    <text>Hvorfor er denne I vores ark?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F831DABE-F25F-40C0-BA60-E859EDB37441}">
-  <dimension ref="A1:G111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AE16E0-6F4D-40C8-B3E7-3817357E19BC}">
+  <dimension ref="B2:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>157</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>158</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>159</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>161</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" t="s">
         <v>162</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
         <v>9662021</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>142</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>110</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>114</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>7310</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
         <v>9769221</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>143</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>110</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>115</v>
       </c>
-      <c r="F3">
+      <c r="G4">
         <v>15400</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
         <v>9745512</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>142</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>110</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="G5">
+        <v>7310</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
         <v>9739496</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>144</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>112</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="G6">
+        <v>13300</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
         <v>9872353</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>144</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>112</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="G7">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
         <v>9308728</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>144</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>110</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="G8">
+        <v>10268</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
         <v>9729740</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>144</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>112</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="G9">
+        <v>13300</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
         <v>9682253</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>142</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>110</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" t="s">
         <v>114</v>
       </c>
-      <c r="F9">
+      <c r="G10">
         <v>7310</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
         <v>9855367</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>144</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>112</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="G11">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
         <v>9729738</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>144</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E12" t="s">
         <v>112</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F12" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="G12">
+        <v>13300</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
         <v>9885910</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C13" t="s">
         <v>144</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
         <v>9214135</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
         <v>144</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E14" t="s">
         <v>110</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F14" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="G14">
+        <v>10268</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
         <v>9228045</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
         <v>144</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E15" t="s">
         <v>110</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="G15">
+        <v>10268</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
         <v>9228057</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C16" t="s">
         <v>144</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E16" t="s">
         <v>110</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F16" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="G16">
+        <v>10268</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="1">
         <v>9861990</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
         <v>144</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E17" t="s">
         <v>112</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F17" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="G17">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="1">
         <v>9304069</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C18" t="s">
         <v>144</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E18" t="s">
         <v>110</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F18" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="G18">
+        <v>10268</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="1">
         <v>9214147</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C19" t="s">
         <v>144</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E19" t="s">
         <v>110</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="G19">
+        <v>7564</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="1">
         <v>9813101</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C20" t="s">
         <v>144</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D20" t="s">
         <v>17</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E20" t="s">
         <v>112</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F20" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="G20">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="1">
         <v>9813113</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" t="s">
         <v>144</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E21" t="s">
         <v>112</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F21" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="G21">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="1">
         <v>9813096</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C22" t="s">
         <v>144</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E22" t="s">
         <v>112</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F22" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="G22">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="1">
         <v>9885908</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C23" t="s">
         <v>144</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="1">
         <v>9447536</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C24" t="s">
         <v>145</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E24" t="s">
         <v>119</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F24" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="G24">
+        <v>29400</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
         <v>9713222</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C25" t="s">
         <v>145</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
         <v>22</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E25" t="s">
         <v>156</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F25" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25">
+      <c r="G25">
+        <v>5690</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
         <v>9866706</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C26" t="s">
         <v>145</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="D25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="1">
         <v>9866691</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C27" t="s">
         <v>145</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="1">
         <v>9745536</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C28" t="s">
         <v>142</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28">
+      <c r="E28" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28">
+        <v>7310</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="1">
         <v>9524982</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
         <v>146</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D29" t="s">
         <v>26</v>
       </c>
-      <c r="D28" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="1">
         <v>9674842</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C30" t="s">
         <v>147</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30">
+      <c r="E30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" t="s">
+        <v>164</v>
+      </c>
+      <c r="G30">
+        <v>12400</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="1">
         <v>9674854</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C31" t="s">
         <v>147</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31">
+      <c r="E31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31">
+        <v>12400</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="1">
         <v>9682265</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C32" t="s">
         <v>142</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
         <v>29</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E32" t="s">
         <v>110</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F32" t="s">
         <v>114</v>
       </c>
-      <c r="F31">
+      <c r="G32">
         <v>7310</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="1">
         <v>9400681</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C33" t="s">
         <v>147</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D33" t="s">
         <v>30</v>
       </c>
-      <c r="D32" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="1">
         <v>9384590</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C34" t="s">
         <v>147</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D34" t="s">
         <v>31</v>
       </c>
-      <c r="D33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" s="1">
         <v>9406013</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C35" t="s">
         <v>147</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" s="1">
         <v>9408205</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C36" t="s">
         <v>147</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="1">
         <v>9406001</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C37" t="s">
         <v>147</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B38" s="1">
         <v>9384605</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C38" t="s">
         <v>147</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D38" t="s">
         <v>35</v>
       </c>
-      <c r="D37" t="s">
-        <v>111</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B39" s="1">
         <v>9410997</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C39" t="s">
         <v>147</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D39" t="s">
         <v>36</v>
       </c>
-      <c r="D38" t="s">
-        <v>111</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B40" s="1">
         <v>9399480</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C40" t="s">
         <v>147</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B41" s="1">
         <v>9320257</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C41" t="s">
         <v>148</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B42" s="1">
         <v>9701358</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C42" t="s">
         <v>147</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B43" s="1">
         <v>9467811</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C43" t="s">
         <v>149</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D43" t="s">
         <v>40</v>
       </c>
-      <c r="D42" t="s">
-        <v>111</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" t="s">
         <v>123</v>
       </c>
-      <c r="F42">
+      <c r="G43">
         <v>13560</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B44" s="1">
         <v>9467809</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C44" t="s">
         <v>149</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D44" t="s">
         <v>41</v>
       </c>
-      <c r="D43" t="s">
-        <v>111</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" t="s">
         <v>123</v>
       </c>
-      <c r="F43">
+      <c r="G44">
         <v>13560</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B45" s="1">
         <v>9467794</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C45" t="s">
         <v>149</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D45" t="s">
         <v>42</v>
       </c>
-      <c r="D44" t="s">
-        <v>111</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F45" t="s">
         <v>123</v>
       </c>
-      <c r="F44">
+      <c r="G45">
         <v>13560</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B46" s="1">
         <v>9856634</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C46" t="s">
         <v>149</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" t="s">
         <v>43</v>
       </c>
-      <c r="D45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" t="s">
         <v>124</v>
       </c>
-      <c r="F45">
+      <c r="G46">
         <v>10850</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B47" s="1">
         <v>9856622</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C47" t="s">
         <v>149</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D47" t="s">
         <v>44</v>
       </c>
-      <c r="D46" t="s">
-        <v>111</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" t="s">
         <v>124</v>
       </c>
-      <c r="F46">
+      <c r="G47">
         <v>10850</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B48" s="1">
         <v>9524994</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C48" t="s">
         <v>146</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D48" t="s">
         <v>45</v>
       </c>
-      <c r="D47" t="s">
-        <v>111</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
+        <v>111</v>
+      </c>
+      <c r="F48" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B49" s="1">
         <v>9483138</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C49" t="s">
         <v>150</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D49" t="s">
         <v>46</v>
       </c>
-      <c r="D48" t="s">
-        <v>111</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
+        <v>111</v>
+      </c>
+      <c r="F49" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B50" s="1">
         <v>9732591</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C50" t="s">
         <v>147</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D50" t="s">
         <v>47</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E50" t="s">
         <v>112</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F50" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B51" s="1">
         <v>9728253</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C51" t="s">
         <v>147</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D51" t="s">
         <v>48</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E51" t="s">
         <v>112</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F51" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B52" s="1">
         <v>9740457</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C52" t="s">
         <v>147</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D52" t="s">
         <v>49</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E52" t="s">
         <v>112</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F52" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B53" s="1">
         <v>9614517</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C53" t="s">
         <v>151</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D53" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B54" s="1">
         <v>9619971</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C54" t="s">
         <v>148</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B55" s="1">
         <v>9166778</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C55" t="s">
         <v>152</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B56" s="1">
         <v>9120841</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C56" t="s">
         <v>152</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D56" t="s">
         <v>53</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E56" t="s">
         <v>110</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F56" t="s">
         <v>127</v>
       </c>
-      <c r="F55">
+      <c r="G56">
         <v>54840</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B57" s="1">
         <v>9662019</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C57" t="s">
         <v>142</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D57" t="s">
         <v>54</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E57" t="s">
         <v>110</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F57" t="s">
         <v>114</v>
       </c>
-      <c r="F56">
+      <c r="G57">
         <v>7310</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B58" s="1">
         <v>9906049</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C58" t="s">
         <v>153</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D58" t="s">
         <v>55</v>
       </c>
-      <c r="D57" t="s">
-        <v>111</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B59" s="1">
         <v>9906037</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C59" t="s">
         <v>153</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D59" t="s">
         <v>56</v>
       </c>
-      <c r="D58" t="s">
-        <v>111</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F59" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B60" s="1">
         <v>9906025</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C60" t="s">
         <v>153</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D60" t="s">
         <v>57</v>
       </c>
-      <c r="D59" t="s">
-        <v>111</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F60" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B61" s="1">
         <v>9906013</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C61" t="s">
         <v>153</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D61" t="s">
         <v>58</v>
       </c>
-      <c r="D60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="E61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F61" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B62" s="1">
         <v>9966233</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C62" t="s">
         <v>153</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D62" t="s">
         <v>59</v>
       </c>
-      <c r="D61" t="s">
-        <v>111</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="E62" t="s">
+        <v>111</v>
+      </c>
+      <c r="F62" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B63" s="1">
         <v>9745524</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C63" t="s">
         <v>142</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D63" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B64" s="1">
         <v>9315446</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C64" t="s">
         <v>146</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D64" t="s">
         <v>61</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E64" t="s">
         <v>110</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F64" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64">
+      <c r="G64">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B65" s="1">
         <v>9401790</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C65" t="s">
         <v>146</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D65" t="s">
         <v>62</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E65" t="s">
         <v>112</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F65" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65">
+      <c r="G65">
+        <v>12268</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B66" s="1">
         <v>9319674</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C66" t="s">
         <v>146</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D66" t="s">
         <v>63</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E66" t="s">
         <v>112</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F66" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66">
+      <c r="G66">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B67" s="1">
         <v>9306639</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C67" t="s">
         <v>146</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D67" t="s">
         <v>64</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E67" t="s">
         <v>113</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F67" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67">
+      <c r="G67">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B68" s="1">
         <v>9283291</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C68" t="s">
         <v>146</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D68" t="s">
         <v>65</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E68" t="s">
         <v>112</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F68" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68">
+      <c r="G68">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B69" s="1">
         <v>9319703</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C69" t="s">
         <v>146</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D69" t="s">
         <v>66</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E69" t="s">
         <v>113</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F69" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69">
+      <c r="G69">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B70" s="1">
         <v>9308948</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C70" t="s">
         <v>146</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D70" t="s">
         <v>67</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E70" t="s">
         <v>112</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F70" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70">
+      <c r="G70">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B71" s="1">
         <v>9308950</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C71" t="s">
         <v>146</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D71" t="s">
         <v>68</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E71" t="s">
         <v>112</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F71" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71">
+      <c r="G71">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B72" s="1">
         <v>9283289</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C72" t="s">
         <v>146</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D72" t="s">
         <v>69</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E72" t="s">
         <v>112</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F72" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72">
+      <c r="G72">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B73" s="1">
         <v>9315458</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C73" t="s">
         <v>146</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D73" t="s">
         <v>70</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E73" t="s">
         <v>112</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F73" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73">
+      <c r="G73">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B74" s="1">
         <v>9598218</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C74" t="s">
         <v>147</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D74" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74">
+      <c r="E74" t="s">
+        <v>112</v>
+      </c>
+      <c r="F74" t="s">
+        <v>167</v>
+      </c>
+      <c r="G74">
+        <v>9760</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B75" s="1">
         <v>9609146</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C75" t="s">
         <v>147</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D75" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75">
+      <c r="E75" t="s">
+        <v>111</v>
+      </c>
+      <c r="F75" t="s">
+        <v>168</v>
+      </c>
+      <c r="G75">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B76" s="1">
         <v>9293583</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C76" t="s">
         <v>147</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D76" t="s">
         <v>73</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E76" t="s">
         <v>156</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F76" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B77" s="1">
         <v>9293909</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C77" t="s">
         <v>147</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D77" t="s">
         <v>74</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E77" t="s">
         <v>156</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F77" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B78" s="1">
         <v>9542984</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C78" t="s">
         <v>154</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D78" t="s">
         <v>75</v>
       </c>
-      <c r="D77" t="s">
-        <v>111</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="E78" t="s">
+        <v>111</v>
+      </c>
+      <c r="F78" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B79" s="1">
         <v>9551777</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C79" t="s">
         <v>154</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D79" t="s">
         <v>76</v>
       </c>
-      <c r="D78" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="E79" t="s">
+        <v>111</v>
+      </c>
+      <c r="F79" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B80" s="1">
         <v>9702209</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C80" t="s">
         <v>155</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D80" t="s">
         <v>77</v>
       </c>
-      <c r="D79" t="s">
-        <v>111</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="E80" t="s">
+        <v>111</v>
+      </c>
+      <c r="F80" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B81" s="1">
         <v>9702194</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C81" t="s">
         <v>155</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D81" t="s">
         <v>78</v>
       </c>
-      <c r="D80" t="s">
-        <v>111</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="E81" t="s">
+        <v>111</v>
+      </c>
+      <c r="F81" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B82" s="1">
         <v>9702211</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C82" t="s">
         <v>155</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D82" t="s">
         <v>79</v>
       </c>
-      <c r="D81" t="s">
-        <v>111</v>
-      </c>
-      <c r="E81" t="s">
+      <c r="E82" t="s">
+        <v>111</v>
+      </c>
+      <c r="F82" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B83" s="1">
         <v>9849992</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C83" t="s">
         <v>155</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D83" t="s">
         <v>80</v>
       </c>
-      <c r="D82" t="s">
-        <v>111</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="E83" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B84" s="1">
         <v>9850006</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C84" t="s">
         <v>155</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D84" t="s">
         <v>81</v>
       </c>
-      <c r="D83" t="s">
-        <v>111</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
+        <v>111</v>
+      </c>
+      <c r="F84" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B85" s="1">
         <v>9712864</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C85" t="s">
         <v>155</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D85" t="s">
         <v>82</v>
       </c>
-      <c r="D84" t="s">
-        <v>111</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="E85" t="s">
+        <v>111</v>
+      </c>
+      <c r="F85" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B86" s="1">
         <v>9904871</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C86" t="s">
         <v>155</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D86" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B87" s="1">
         <v>9798002</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C87" t="s">
         <v>155</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D87" t="s">
         <v>84</v>
       </c>
-      <c r="D86" t="s">
-        <v>111</v>
-      </c>
-      <c r="E86" t="s">
+      <c r="E87" t="s">
+        <v>111</v>
+      </c>
+      <c r="F87" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B88" s="1">
         <v>9797981</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C88" t="s">
         <v>155</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D88" t="s">
         <v>85</v>
       </c>
-      <c r="D87" t="s">
-        <v>111</v>
-      </c>
-      <c r="E87" t="s">
+      <c r="E88" t="s">
+        <v>111</v>
+      </c>
+      <c r="F88" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B89" s="1">
         <v>9797993</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C89" t="s">
         <v>155</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D89" t="s">
         <v>86</v>
       </c>
-      <c r="D88" t="s">
-        <v>111</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="E89" t="s">
+        <v>111</v>
+      </c>
+      <c r="F89" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B90" s="1">
         <v>9798014</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C90" t="s">
         <v>155</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D90" t="s">
         <v>87</v>
       </c>
-      <c r="D89" t="s">
-        <v>111</v>
-      </c>
-      <c r="E89" t="s">
+      <c r="E90" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B91" s="1">
         <v>9904883</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C91" t="s">
         <v>155</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D91" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B92" s="1">
         <v>9701554</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C92" t="s">
         <v>155</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D92" t="s">
         <v>89</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E92" t="s">
         <v>112</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F92" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B93" s="1">
         <v>9701566</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C93" t="s">
         <v>155</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D93" t="s">
         <v>90</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E93" t="s">
         <v>112</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F93" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A93">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B94" s="1">
         <v>9694646</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C94" t="s">
         <v>155</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D94" t="s">
         <v>91</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E94" t="s">
         <v>112</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F94" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A94">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B95" s="1">
         <v>9375616</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C95" t="s">
         <v>155</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D95" t="s">
         <v>92</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E95" t="s">
         <v>112</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F95" t="s">
         <v>138</v>
       </c>
-      <c r="F94">
+      <c r="G95">
         <v>11340</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A95">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B96" s="1">
         <v>9390769</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C96" t="s">
         <v>155</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D96" t="s">
         <v>93</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E96" t="s">
         <v>112</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F96" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A96">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B97" s="1">
         <v>9392470</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C97" t="s">
         <v>155</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D97" t="s">
         <v>94</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E97" t="s">
         <v>112</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F97" t="s">
         <v>138</v>
       </c>
-      <c r="F96">
+      <c r="G97">
         <v>11340</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A97">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B98" s="1">
         <v>9392468</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C98" t="s">
         <v>155</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D98" t="s">
         <v>95</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E98" t="s">
         <v>112</v>
       </c>
-      <c r="E97" t="s">
+      <c r="F98" t="s">
         <v>138</v>
       </c>
-      <c r="F97">
+      <c r="G98">
         <v>11620</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A98">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B99" s="1">
         <v>9392482</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C99" t="s">
         <v>155</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D99" t="s">
         <v>96</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E99" t="s">
         <v>112</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F99" t="s">
         <v>138</v>
       </c>
-      <c r="F98">
+      <c r="G99">
         <v>11620</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A99">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B100" s="1">
         <v>9836050</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C100" t="s">
         <v>155</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D100" t="s">
         <v>97</v>
       </c>
-      <c r="D99" t="s">
-        <v>111</v>
-      </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
+        <v>111</v>
+      </c>
+      <c r="F100" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A100">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B101" s="1">
         <v>9797723</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C101" t="s">
         <v>155</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D101" t="s">
         <v>98</v>
       </c>
-      <c r="D100" t="s">
-        <v>111</v>
-      </c>
-      <c r="E100" t="s">
+      <c r="E101" t="s">
+        <v>111</v>
+      </c>
+      <c r="F101" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A101">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B102" s="1">
         <v>9854791</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C102" t="s">
         <v>155</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D102" t="s">
         <v>99</v>
       </c>
-      <c r="D101" t="s">
-        <v>111</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="E102" t="s">
+        <v>111</v>
+      </c>
+      <c r="F102" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A102">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B103" s="1">
         <v>9854806</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C103" t="s">
         <v>155</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D103" t="s">
         <v>100</v>
       </c>
-      <c r="D102" t="s">
-        <v>111</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="E103" t="s">
+        <v>111</v>
+      </c>
+      <c r="F103" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A103">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B104" s="1">
         <v>9836036</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C104" t="s">
         <v>155</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D104" t="s">
         <v>101</v>
       </c>
-      <c r="D103" t="s">
-        <v>111</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="E104" t="s">
+        <v>111</v>
+      </c>
+      <c r="F104" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A104">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B105" s="1">
         <v>9836062</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C105" t="s">
         <v>155</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D105" t="s">
         <v>102</v>
       </c>
-      <c r="D104" t="s">
-        <v>111</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="E105" t="s">
+        <v>111</v>
+      </c>
+      <c r="F105" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A105">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B106" s="1">
         <v>9854789</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C106" t="s">
         <v>155</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D106" t="s">
         <v>103</v>
       </c>
-      <c r="D105" t="s">
-        <v>111</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="E106" t="s">
+        <v>111</v>
+      </c>
+      <c r="F106" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A106">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B107" s="1">
         <v>9836048</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C107" t="s">
         <v>155</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D107" t="s">
         <v>104</v>
       </c>
-      <c r="D106" t="s">
-        <v>111</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="E107" t="s">
+        <v>111</v>
+      </c>
+      <c r="F107" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A107">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B108" s="1">
         <v>9797735</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C108" t="s">
         <v>155</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D108" t="s">
         <v>105</v>
       </c>
-      <c r="D107" t="s">
-        <v>111</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="E108" t="s">
+        <v>111</v>
+      </c>
+      <c r="F108" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A108">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B109" s="1">
         <v>9712319</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C109" t="s">
         <v>155</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D109" t="s">
         <v>106</v>
       </c>
-      <c r="D108" t="s">
-        <v>111</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="E109" t="s">
+        <v>111</v>
+      </c>
+      <c r="F109" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A109">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B110" s="1">
         <v>9712321</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C110" t="s">
         <v>155</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D110" t="s">
         <v>107</v>
       </c>
-      <c r="D109" t="s">
-        <v>111</v>
-      </c>
-      <c r="E109" t="s">
+      <c r="E110" t="s">
+        <v>111</v>
+      </c>
+      <c r="F110" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A110">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B111" s="1">
         <v>9726475</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C111" t="s">
         <v>155</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D111" t="s">
         <v>108</v>
       </c>
-      <c r="D110" t="s">
-        <v>111</v>
-      </c>
-      <c r="E110" t="s">
+      <c r="E111" t="s">
+        <v>111</v>
+      </c>
+      <c r="F111" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A111">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B112" s="1">
         <v>9775737</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C112" t="s">
         <v>148</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D112" t="s">
         <v>109</v>
       </c>
+      <c r="E112" t="s">
+        <v>111</v>
+      </c>
+      <c r="F112" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F831DABE-F25F-40C0-BA60-E859EDB37441}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e92f16c9-db69-4522-84e2-bf933696a321" xsi:nil="true"/>
+    <_x0031_0 xmlns="6e040d9b-4d00-4c60-b912-ca778ccae294" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6e040d9b-4d00-4c60-b912-ca778ccae294">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000B73ECAA2334A14EB365ED6608A878E1" ma:contentTypeVersion="20" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="3a0a8eb6936e710403338e49b0d9cf8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6e040d9b-4d00-4c60-b912-ca778ccae294" xmlns:ns3="e92f16c9-db69-4522-84e2-bf933696a321" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="879cce07b0e372e82448d845ce3e64df" ns2:_="" ns3:_="">
     <xsd:import namespace="6e040d9b-4d00-4c60-b912-ca778ccae294"/>
@@ -3004,28 +3336,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e92f16c9-db69-4522-84e2-bf933696a321" xsi:nil="true"/>
-    <_x0031_0 xmlns="6e040d9b-4d00-4c60-b912-ca778ccae294" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6e040d9b-4d00-4c60-b912-ca778ccae294">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABB72383-3208-4DA4-A3CB-6496336595CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e92f16c9-db69-4522-84e2-bf933696a321"/>
+    <ds:schemaRef ds:uri="6e040d9b-4d00-4c60-b912-ca778ccae294"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{855F6443-400B-4276-AA3F-D8A900D50BF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3719BABF-6018-4300-8EF8-A21D23A9485A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3042,23 +3372,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABB72383-3208-4DA4-A3CB-6496336595CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e92f16c9-db69-4522-84e2-bf933696a321"/>
-    <ds:schemaRef ds:uri="6e040d9b-4d00-4c60-b912-ca778ccae294"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{855F6443-400B-4276-AA3F-D8A900D50BF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated ME and MCR and moved app and index
</commit_message>
<xml_diff>
--- a/Legacy data vessels.xlsx
+++ b/Legacy data vessels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid.sharepoint.com/sites/MarineFluidTechnologyAS/Shared Documents/Projects/16. Feedback report to vessels/Feedback report generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3B07B958-9481-4337-BE77-39E9672A75B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A96CFDC6-F699-4382-8669-A552CBE0733F}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{3B07B958-9481-4337-BE77-39E9672A75B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDFA7025-0413-4F08-8A58-F36E5E759738}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="9750" windowHeight="10155" xr2:uid="{9994A8F6-3190-471E-B791-9B9DB550B49C}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{9994A8F6-3190-471E-B791-9B9DB550B49C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="175">
   <si>
     <t>Adriatic Gas</t>
   </si>
@@ -543,6 +543,24 @@
   </si>
   <si>
     <t>5S46MC-C</t>
+  </si>
+  <si>
+    <t>7S80MC</t>
+  </si>
+  <si>
+    <t>6S70MC-C7</t>
+  </si>
+  <si>
+    <t>6RT-flex58T</t>
+  </si>
+  <si>
+    <t>MSC Yukta</t>
+  </si>
+  <si>
+    <t>7S90MC-C7</t>
+  </si>
+  <si>
+    <t>7S65ME</t>
   </si>
 </sst>
 </file>
@@ -595,10 +613,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,13 +932,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F831DABE-F25F-40C0-BA60-E859EDB37441}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
@@ -935,7 +949,7 @@
     <col min="7" max="7" width="5.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>157</v>
       </c>
@@ -958,7 +972,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>9662021</v>
       </c>
@@ -978,7 +992,7 @@
         <v>7310</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9769221</v>
       </c>
@@ -998,7 +1012,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>9745512</v>
       </c>
@@ -1018,7 +1032,7 @@
         <v>7310</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>9739496</v>
       </c>
@@ -1038,7 +1052,7 @@
         <v>13300</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>9872353</v>
       </c>
@@ -1058,7 +1072,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>9308728</v>
       </c>
@@ -1078,7 +1092,7 @@
         <v>10268</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9729740</v>
       </c>
@@ -1098,7 +1112,7 @@
         <v>13300</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9682253</v>
       </c>
@@ -1118,7 +1132,7 @@
         <v>7310</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9855367</v>
       </c>
@@ -1138,7 +1152,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9729738</v>
       </c>
@@ -1158,7 +1172,7 @@
         <v>13300</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9885910</v>
       </c>
@@ -1169,7 +1183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>9214135</v>
       </c>
@@ -1189,7 +1203,7 @@
         <v>10268</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>9228045</v>
       </c>
@@ -1209,7 +1223,7 @@
         <v>10268</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>9228057</v>
       </c>
@@ -1229,7 +1243,7 @@
         <v>10268</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>9861990</v>
       </c>
@@ -1249,7 +1263,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>9304069</v>
       </c>
@@ -1269,7 +1283,7 @@
         <v>10268</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9214147</v>
       </c>
@@ -1289,7 +1303,7 @@
         <v>7564</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>9813101</v>
       </c>
@@ -1309,7 +1323,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>9813113</v>
       </c>
@@ -1329,7 +1343,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9813096</v>
       </c>
@@ -1349,7 +1363,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>9885908</v>
       </c>
@@ -1360,7 +1374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>9447536</v>
       </c>
@@ -1380,7 +1394,7 @@
         <v>29400</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>9713222</v>
       </c>
@@ -1400,7 +1414,7 @@
         <v>5690</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>9866706</v>
       </c>
@@ -1417,7 +1431,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>9866691</v>
       </c>
@@ -1428,7 +1442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>9745536</v>
       </c>
@@ -1448,7 +1462,7 @@
         <v>7310</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>9524982</v>
       </c>
@@ -1465,7 +1479,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>9674842</v>
       </c>
@@ -1485,7 +1499,7 @@
         <v>12400</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>9674854</v>
       </c>
@@ -1505,7 +1519,7 @@
         <v>12400</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>9682265</v>
       </c>
@@ -1525,7 +1539,7 @@
         <v>7310</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>9400681</v>
       </c>
@@ -1541,8 +1555,11 @@
       <c r="E32" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F32">
+        <v>25480</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>9384590</v>
       </c>
@@ -1558,8 +1575,11 @@
       <c r="E33" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F33">
+        <v>25480</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>9406013</v>
       </c>
@@ -1569,8 +1589,17 @@
       <c r="C34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34">
+        <v>10394</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>9408205</v>
       </c>
@@ -1580,8 +1609,17 @@
       <c r="C35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D35" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35">
+        <v>10394</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>9406001</v>
       </c>
@@ -1591,8 +1629,17 @@
       <c r="C36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36">
+        <v>10394</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>9384605</v>
       </c>
@@ -1606,10 +1653,13 @@
         <v>111</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
+        <v>173</v>
+      </c>
+      <c r="F37">
+        <v>25480</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>9410997</v>
       </c>
@@ -1625,8 +1675,11 @@
       <c r="E38" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F38">
+        <v>25480</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>9399480</v>
       </c>
@@ -1636,8 +1689,17 @@
       <c r="C39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39">
+        <v>10394</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>9320257</v>
       </c>
@@ -1647,8 +1709,14 @@
       <c r="C40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>9701358</v>
       </c>
@@ -1658,8 +1726,17 @@
       <c r="C41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41">
+        <v>15860</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>9467811</v>
       </c>
@@ -1679,7 +1756,7 @@
         <v>13560</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>9467809</v>
       </c>
@@ -1699,7 +1776,7 @@
         <v>13560</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>9467794</v>
       </c>
@@ -1719,7 +1796,7 @@
         <v>13560</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>9856634</v>
       </c>
@@ -1739,7 +1816,7 @@
         <v>10850</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>9856622</v>
       </c>
@@ -1759,7 +1836,7 @@
         <v>10850</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>9524994</v>
       </c>
@@ -1776,7 +1853,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>9483138</v>
       </c>
@@ -1792,8 +1869,11 @@
       <c r="E48" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F48">
+        <v>18660</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>9732591</v>
       </c>
@@ -1809,8 +1889,11 @@
       <c r="E49" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F49">
+        <v>36870</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>9728253</v>
       </c>
@@ -1826,8 +1909,11 @@
       <c r="E50" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F50">
+        <v>37200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>9740457</v>
       </c>
@@ -1843,8 +1929,11 @@
       <c r="E51" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F51">
+        <v>36870</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>9614517</v>
       </c>
@@ -1854,8 +1943,17 @@
       <c r="C52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D52" t="s">
+        <v>112</v>
+      </c>
+      <c r="E52" t="s">
+        <v>171</v>
+      </c>
+      <c r="F52">
+        <v>13560</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>9619971</v>
       </c>
@@ -1866,7 +1964,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>9166778</v>
       </c>
@@ -1876,8 +1974,17 @@
       <c r="C54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="D54" t="s">
+        <v>110</v>
+      </c>
+      <c r="E54" t="s">
+        <v>127</v>
+      </c>
+      <c r="F54">
+        <v>54840</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>9120841</v>
       </c>
@@ -1897,52 +2004,55 @@
         <v>54840</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>9662019</v>
+        <v>9146467</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
       <c r="D56" t="s">
         <v>110</v>
       </c>
       <c r="E56" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56">
+        <v>54840</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>9662019</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" t="s">
+        <v>110</v>
+      </c>
+      <c r="E57" t="s">
         <v>114</v>
       </c>
-      <c r="F56">
+      <c r="F57">
         <v>7310</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A57">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58">
         <v>9906049</v>
-      </c>
-      <c r="B57" t="s">
-        <v>153</v>
-      </c>
-      <c r="C57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" t="s">
-        <v>111</v>
-      </c>
-      <c r="E57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A58">
-        <v>9906037</v>
       </c>
       <c r="B58" t="s">
         <v>153</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" t="s">
         <v>111</v>
@@ -1950,16 +2060,19 @@
       <c r="E58" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F58">
+        <v>7310</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>9906025</v>
+        <v>9906037</v>
       </c>
       <c r="B59" t="s">
         <v>153</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D59" t="s">
         <v>111</v>
@@ -1967,16 +2080,19 @@
       <c r="E59" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F59">
+        <v>15750</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>9906013</v>
+        <v>9906025</v>
       </c>
       <c r="B60" t="s">
         <v>153</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" t="s">
         <v>111</v>
@@ -1984,84 +2100,99 @@
       <c r="E60" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F60">
+        <v>23542</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>9966233</v>
+        <v>9906013</v>
       </c>
       <c r="B61" t="s">
         <v>153</v>
       </c>
       <c r="C61" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" t="s">
+        <v>111</v>
+      </c>
+      <c r="E61" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61">
+        <v>15742</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>9966233</v>
+      </c>
+      <c r="B62" t="s">
+        <v>153</v>
+      </c>
+      <c r="C62" t="s">
         <v>59</v>
       </c>
-      <c r="D61" t="s">
-        <v>111</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="D62" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A62">
+      <c r="F62">
+        <v>11400</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63">
         <v>9745524</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>142</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A63">
+      <c r="D63" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" t="s">
+        <v>164</v>
+      </c>
+      <c r="F63">
+        <v>9960</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64">
         <v>9315446</v>
-      </c>
-      <c r="B63" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" t="s">
-        <v>61</v>
-      </c>
-      <c r="D63" t="s">
-        <v>110</v>
-      </c>
-      <c r="E63" t="s">
-        <v>130</v>
-      </c>
-      <c r="F63">
-        <v>15540</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A64">
-        <v>9401790</v>
       </c>
       <c r="B64" t="s">
         <v>146</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F64">
-        <v>12268</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>9319674</v>
+        <v>9401790</v>
       </c>
       <c r="B65" t="s">
         <v>146</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" t="s">
         <v>112</v>
@@ -2070,215 +2201,218 @@
         <v>131</v>
       </c>
       <c r="F65">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.75">
+        <v>12268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>9306639</v>
+        <v>9319674</v>
       </c>
       <c r="B66" t="s">
         <v>146</v>
       </c>
       <c r="C66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F66">
         <v>15260</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>9283291</v>
+        <v>9306639</v>
       </c>
       <c r="B67" t="s">
         <v>146</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E67" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F67">
-        <v>15540</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>9319703</v>
+        <v>9283291</v>
       </c>
       <c r="B68" t="s">
         <v>146</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F68">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>9308948</v>
+        <v>9319703</v>
       </c>
       <c r="B69" t="s">
         <v>146</v>
       </c>
       <c r="C69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E69" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F69">
-        <v>15540</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>9308950</v>
+        <v>9308948</v>
       </c>
       <c r="B70" t="s">
         <v>146</v>
       </c>
       <c r="C70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D70" t="s">
         <v>112</v>
       </c>
       <c r="E70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F70">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>9283289</v>
+        <v>9308950</v>
       </c>
       <c r="B71" t="s">
         <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D71" t="s">
         <v>112</v>
       </c>
       <c r="E71" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F71">
-        <v>15540</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>9315458</v>
+        <v>9283289</v>
       </c>
       <c r="B72" t="s">
         <v>146</v>
       </c>
       <c r="C72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D72" t="s">
         <v>112</v>
       </c>
       <c r="E72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F72">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>9598218</v>
+        <v>9315458</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
         <v>112</v>
       </c>
       <c r="E73" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="F73">
-        <v>9760</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.75">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>9609146</v>
+        <v>9598218</v>
       </c>
       <c r="B74" t="s">
         <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D74" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F74">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.75">
+        <v>9760</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>9293583</v>
+        <v>9609146</v>
       </c>
       <c r="B75" t="s">
         <v>147</v>
       </c>
       <c r="C75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D75" t="s">
-        <v>156</v>
+        <v>111</v>
       </c>
       <c r="E75" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.75">
+        <v>168</v>
+      </c>
+      <c r="F75">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>9293909</v>
+        <v>9293583</v>
       </c>
       <c r="B76" t="s">
         <v>147</v>
       </c>
       <c r="C76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D76" t="s">
         <v>156</v>
@@ -2286,67 +2420,73 @@
       <c r="E76" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F76">
+        <v>15130</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
+        <v>9293909</v>
+      </c>
+      <c r="B77" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" t="s">
+        <v>74</v>
+      </c>
+      <c r="D77" t="s">
+        <v>156</v>
+      </c>
+      <c r="E77" t="s">
+        <v>133</v>
+      </c>
+      <c r="F77">
+        <v>15090</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78">
         <v>9542984</v>
-      </c>
-      <c r="B77" t="s">
-        <v>154</v>
-      </c>
-      <c r="C77" t="s">
-        <v>75</v>
-      </c>
-      <c r="D77" t="s">
-        <v>111</v>
-      </c>
-      <c r="E77" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A78">
-        <v>9551777</v>
       </c>
       <c r="B78" t="s">
         <v>154</v>
       </c>
       <c r="C78" t="s">
+        <v>75</v>
+      </c>
+      <c r="D78" t="s">
+        <v>111</v>
+      </c>
+      <c r="E78" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>9551777</v>
+      </c>
+      <c r="B79" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" t="s">
         <v>76</v>
       </c>
-      <c r="D78" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="D79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E79" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A79">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80">
         <v>9702209</v>
-      </c>
-      <c r="B79" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" t="s">
-        <v>77</v>
-      </c>
-      <c r="D79" t="s">
-        <v>111</v>
-      </c>
-      <c r="E79" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A80">
-        <v>9702194</v>
       </c>
       <c r="B80" t="s">
         <v>155</v>
       </c>
       <c r="C80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D80" t="s">
         <v>111</v>
@@ -2355,15 +2495,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>9702211</v>
+        <v>9702194</v>
       </c>
       <c r="B81" t="s">
         <v>155</v>
       </c>
       <c r="C81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D81" t="s">
         <v>111</v>
@@ -2372,15 +2512,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>9849992</v>
+        <v>9702211</v>
       </c>
       <c r="B82" t="s">
         <v>155</v>
       </c>
       <c r="C82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D82" t="s">
         <v>111</v>
@@ -2389,15 +2529,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>9850006</v>
+        <v>9849992</v>
       </c>
       <c r="B83" t="s">
         <v>155</v>
       </c>
       <c r="C83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D83" t="s">
         <v>111</v>
@@ -2406,60 +2546,63 @@
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>9712864</v>
+        <v>9850006</v>
       </c>
       <c r="B84" t="s">
         <v>155</v>
       </c>
       <c r="C84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
       </c>
       <c r="E84" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>9904871</v>
+        <v>9712864</v>
       </c>
       <c r="B85" t="s">
         <v>155</v>
       </c>
       <c r="C85" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.75">
+        <v>82</v>
+      </c>
+      <c r="D85" t="s">
+        <v>111</v>
+      </c>
+      <c r="E85" t="s">
+        <v>137</v>
+      </c>
+      <c r="F85">
+        <v>14280</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>9798002</v>
+        <v>9904871</v>
       </c>
       <c r="B86" t="s">
         <v>155</v>
       </c>
       <c r="C86" t="s">
-        <v>84</v>
-      </c>
-      <c r="D86" t="s">
-        <v>111</v>
-      </c>
-      <c r="E86" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>9797981</v>
+        <v>9798002</v>
       </c>
       <c r="B87" t="s">
         <v>155</v>
       </c>
       <c r="C87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D87" t="s">
         <v>111</v>
@@ -2468,15 +2611,15 @@
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>9797993</v>
+        <v>9797981</v>
       </c>
       <c r="B88" t="s">
         <v>155</v>
       </c>
       <c r="C88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88" t="s">
         <v>111</v>
@@ -2485,15 +2628,15 @@
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>9798014</v>
+        <v>9797993</v>
       </c>
       <c r="B89" t="s">
         <v>155</v>
       </c>
       <c r="C89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D89" t="s">
         <v>111</v>
@@ -2502,43 +2645,43 @@
         <v>137</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>9904883</v>
+        <v>9798014</v>
       </c>
       <c r="B90" t="s">
         <v>155</v>
       </c>
       <c r="C90" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.75">
+        <v>87</v>
+      </c>
+      <c r="D90" t="s">
+        <v>111</v>
+      </c>
+      <c r="E90" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>9701554</v>
+        <v>9904883</v>
       </c>
       <c r="B91" t="s">
         <v>155</v>
       </c>
       <c r="C91" t="s">
-        <v>89</v>
-      </c>
-      <c r="D91" t="s">
-        <v>112</v>
-      </c>
-      <c r="E91" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.75">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>9701566</v>
+        <v>9701554</v>
       </c>
       <c r="B92" t="s">
         <v>155</v>
       </c>
       <c r="C92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D92" t="s">
         <v>112</v>
@@ -2547,15 +2690,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>9694646</v>
+        <v>9701566</v>
       </c>
       <c r="B93" t="s">
         <v>155</v>
       </c>
       <c r="C93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D93" t="s">
         <v>112</v>
@@ -2564,35 +2707,32 @@
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>9375616</v>
+        <v>9694646</v>
       </c>
       <c r="B94" t="s">
         <v>155</v>
       </c>
       <c r="C94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D94" t="s">
         <v>112</v>
       </c>
       <c r="E94" t="s">
-        <v>138</v>
-      </c>
-      <c r="F94">
-        <v>11340</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.75">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>9390769</v>
+        <v>9375616</v>
       </c>
       <c r="B95" t="s">
         <v>155</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D95" t="s">
         <v>112</v>
@@ -2600,16 +2740,19 @@
       <c r="E95" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="F95">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>9392470</v>
+        <v>9390769</v>
       </c>
       <c r="B96" t="s">
         <v>155</v>
       </c>
       <c r="C96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96" t="s">
         <v>112</v>
@@ -2617,19 +2760,16 @@
       <c r="E96" t="s">
         <v>138</v>
       </c>
-      <c r="F96">
-        <v>11340</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.75">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>9392468</v>
+        <v>9392470</v>
       </c>
       <c r="B97" t="s">
         <v>155</v>
       </c>
       <c r="C97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D97" t="s">
         <v>112</v>
@@ -2638,18 +2778,18 @@
         <v>138</v>
       </c>
       <c r="F97">
-        <v>11620</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.75">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>9392482</v>
+        <v>9392468</v>
       </c>
       <c r="B98" t="s">
         <v>155</v>
       </c>
       <c r="C98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D98" t="s">
         <v>112</v>
@@ -2661,66 +2801,69 @@
         <v>11620</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>9836050</v>
+        <v>9392482</v>
       </c>
       <c r="B99" t="s">
         <v>155</v>
       </c>
       <c r="C99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D99" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E99" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+      <c r="F99">
+        <v>11620</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>9797723</v>
+        <v>9836050</v>
       </c>
       <c r="B100" t="s">
         <v>155</v>
       </c>
       <c r="C100" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D100" t="s">
         <v>111</v>
       </c>
       <c r="E100" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>9854791</v>
+        <v>9797723</v>
       </c>
       <c r="B101" t="s">
         <v>155</v>
       </c>
       <c r="C101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D101" t="s">
         <v>111</v>
       </c>
       <c r="E101" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.75">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>9854806</v>
+        <v>9854791</v>
       </c>
       <c r="B102" t="s">
         <v>155</v>
       </c>
       <c r="C102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D102" t="s">
         <v>111</v>
@@ -2729,15 +2872,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>9836036</v>
+        <v>9854806</v>
       </c>
       <c r="B103" t="s">
         <v>155</v>
       </c>
       <c r="C103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D103" t="s">
         <v>111</v>
@@ -2746,15 +2889,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>9836062</v>
+        <v>9836036</v>
       </c>
       <c r="B104" t="s">
         <v>155</v>
       </c>
       <c r="C104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D104" t="s">
         <v>111</v>
@@ -2763,15 +2906,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>9854789</v>
+        <v>9836062</v>
       </c>
       <c r="B105" t="s">
         <v>155</v>
       </c>
       <c r="C105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D105" t="s">
         <v>111</v>
@@ -2780,15 +2923,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>9836048</v>
+        <v>9854789</v>
       </c>
       <c r="B106" t="s">
         <v>155</v>
       </c>
       <c r="C106" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D106" t="s">
         <v>111</v>
@@ -2797,32 +2940,32 @@
         <v>136</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>9797735</v>
+        <v>9836048</v>
       </c>
       <c r="B107" t="s">
         <v>155</v>
       </c>
       <c r="C107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D107" t="s">
         <v>111</v>
       </c>
       <c r="E107" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>9712319</v>
+        <v>9797735</v>
       </c>
       <c r="B108" t="s">
         <v>155</v>
       </c>
       <c r="C108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D108" t="s">
         <v>111</v>
@@ -2831,15 +2974,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>9712321</v>
+        <v>9712319</v>
       </c>
       <c r="B109" t="s">
         <v>155</v>
       </c>
       <c r="C109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2848,15 +2991,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>9726475</v>
+        <v>9712321</v>
       </c>
       <c r="B110" t="s">
         <v>155</v>
       </c>
       <c r="C110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D110" t="s">
         <v>111</v>
@@ -2865,20 +3008,37 @@
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
+        <v>9726475</v>
+      </c>
+      <c r="B111" t="s">
+        <v>155</v>
+      </c>
+      <c r="C111" t="s">
+        <v>108</v>
+      </c>
+      <c r="D111" t="s">
+        <v>111</v>
+      </c>
+      <c r="E111" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112">
         <v>9775737</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>148</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>109</v>
       </c>
-      <c r="D111" t="s">
-        <v>111</v>
-      </c>
-      <c r="E111" t="s">
+      <c r="D112" t="s">
+        <v>111</v>
+      </c>
+      <c r="E112" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Updated Legacy Data Vessels.xlsx"
</commit_message>
<xml_diff>
--- a/Legacy data vessels.xlsx
+++ b/Legacy data vessels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid.sharepoint.com/sites/MarineFluidTechnologyAS/Shared Documents/Projects/16. Feedback report to vessels/Feedback report generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{3B07B958-9481-4337-BE77-39E9672A75B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F6FDDC4-22B7-40F4-9112-9DB0871F8703}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{3B07B958-9481-4337-BE77-39E9672A75B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D4E27E2-EE89-45F8-AE81-9DA203657A8F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="51420" windowHeight="13900" xr2:uid="{9994A8F6-3190-471E-B791-9B9DB550B49C}"/>
+    <workbookView xWindow="-78" yWindow="0" windowWidth="11676" windowHeight="12318" xr2:uid="{9994A8F6-3190-471E-B791-9B9DB550B49C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="195">
   <si>
     <t>Adriatic Gas</t>
   </si>
@@ -362,9 +362,6 @@
     <t>TORM Torino</t>
   </si>
   <si>
-    <t>TORM Troilus</t>
-  </si>
-  <si>
     <t>Vistula Maersk</t>
   </si>
   <si>
@@ -554,9 +551,6 @@
     <t>6RT-flex58T</t>
   </si>
   <si>
-    <t>MSC Yukta</t>
-  </si>
-  <si>
     <t>7S90MC-C7</t>
   </si>
   <si>
@@ -569,7 +563,64 @@
     <t>12RT-flex96C</t>
   </si>
   <si>
-    <t>BSM</t>
+    <t>Hafnia Leo</t>
+  </si>
+  <si>
+    <t>Hafnia Tauras</t>
+  </si>
+  <si>
+    <t>MSC Bremerhaven V</t>
+  </si>
+  <si>
+    <t>MSC Chiara X</t>
+  </si>
+  <si>
+    <t>MSC Denisse X</t>
+  </si>
+  <si>
+    <t>MSC Ellen</t>
+  </si>
+  <si>
+    <t>MSC FIE X</t>
+  </si>
+  <si>
+    <t>MSC Giovanna VII</t>
+  </si>
+  <si>
+    <t>MSC Iniya V</t>
+  </si>
+  <si>
+    <t>MSC Jasmin X</t>
+  </si>
+  <si>
+    <t>MSC Leandra V</t>
+  </si>
+  <si>
+    <t>MSC Nicole X</t>
+  </si>
+  <si>
+    <t>MSC Rita V</t>
+  </si>
+  <si>
+    <t>MSC Vilda X</t>
+  </si>
+  <si>
+    <t>MSC Yukta X</t>
+  </si>
+  <si>
+    <t>Torm Trouilus</t>
+  </si>
+  <si>
+    <t>6S50MC-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6S50MC-C </t>
+  </si>
+  <si>
+    <t>6G50ME-C9.6</t>
+  </si>
+  <si>
+    <t>6G50ME-C9.11</t>
   </si>
 </sst>
 </file>
@@ -622,6 +673,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -941,2215 +996,2435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F831DABE-F25F-40C0-BA60-E859EDB37441}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.47265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
         <v>157</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>158</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>159</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>161</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>162</v>
       </c>
-      <c r="G1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>9662021</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F2">
         <v>7310</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>9769221</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3">
         <v>15400</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>9745512</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F4">
         <v>7310</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>9739496</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F5">
         <v>13300</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>9872353</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6">
         <v>9600</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>9308728</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F7">
         <v>10268</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>9729740</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F8">
         <v>13300</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>9682253</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9">
         <v>7310</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9855367</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10">
         <v>9600</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>9729738</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11">
         <v>13300</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>9885910</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>9214135</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F13">
         <v>10268</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>9228045</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F14">
         <v>10268</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>9228057</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15">
         <v>10268</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>9861990</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F16">
         <v>9600</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>9304069</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17">
         <v>10268</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>9214147</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18">
         <v>7564</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>9813101</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F19">
         <v>9600</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>9813113</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F20">
         <v>9600</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>9813096</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F21">
         <v>9600</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>9885908</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>9447536</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F23">
         <v>29400</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>9713222</v>
       </c>
       <c r="B24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F24">
         <v>5690</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>9866706</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>9866691</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>9745536</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F27">
         <v>7310</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>9524982</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C28" t="s">
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F28">
         <v>12350</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>9674842</v>
       </c>
       <c r="B29" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F29">
         <v>12400</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>9674854</v>
       </c>
       <c r="B30" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F30">
         <v>12400</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>9682265</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F31">
         <v>7310</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>9400681</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F32">
         <v>25480</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>9384590</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F33">
         <v>25480</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>9406013</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F34">
         <v>10394</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>9408205</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F35">
         <v>10394</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>9406001</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F36">
         <v>10394</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>9384605</v>
       </c>
       <c r="B37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C37" t="s">
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F37">
         <v>25480</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>9410997</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F38">
         <v>25480</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>9399480</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F39">
         <v>10394</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>9320257</v>
       </c>
       <c r="B40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F40">
         <v>68658</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>9701358</v>
       </c>
       <c r="B41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
         <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F41">
         <v>15860</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>9467811</v>
       </c>
       <c r="B42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F42">
         <v>13560</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>9467809</v>
       </c>
       <c r="B43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F43">
         <v>13560</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>9467794</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C44" t="s">
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F44">
         <v>13560</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>9856634</v>
       </c>
       <c r="B45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
         <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F45">
         <v>10850</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>9856622</v>
       </c>
       <c r="B46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
         <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F46">
         <v>10850</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
+        <v>9476824</v>
+      </c>
+      <c r="B47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" t="s">
+        <v>175</v>
+      </c>
+      <c r="D47" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" t="s">
+        <v>191</v>
+      </c>
+      <c r="F47">
+        <v>12880</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>9461673</v>
+      </c>
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>176</v>
+      </c>
+      <c r="D48" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" t="s">
+        <v>192</v>
+      </c>
+      <c r="F48">
+        <v>12880</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
         <v>9524994</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="s">
+        <v>110</v>
+      </c>
+      <c r="E49" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49">
+        <v>12350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>9483138</v>
+      </c>
+      <c r="B50" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50">
+        <v>18660</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>9732591</v>
+      </c>
+      <c r="B51" t="s">
         <v>146</v>
       </c>
-      <c r="C47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" t="s">
         <v>111</v>
       </c>
-      <c r="E47" t="s">
-        <v>141</v>
-      </c>
-      <c r="F47">
-        <v>12350</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>9483138</v>
-      </c>
-      <c r="B48" t="s">
-        <v>150</v>
-      </c>
-      <c r="C48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" t="s">
-        <v>111</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="E51" t="s">
         <v>125</v>
-      </c>
-      <c r="F48">
-        <v>18660</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>9732591</v>
-      </c>
-      <c r="B49" t="s">
-        <v>177</v>
-      </c>
-      <c r="C49" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49" t="s">
-        <v>112</v>
-      </c>
-      <c r="E49" t="s">
-        <v>126</v>
-      </c>
-      <c r="F49">
-        <v>36870</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>9728253</v>
-      </c>
-      <c r="B50" t="s">
-        <v>177</v>
-      </c>
-      <c r="C50" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" t="s">
-        <v>112</v>
-      </c>
-      <c r="E50" t="s">
-        <v>126</v>
-      </c>
-      <c r="F50">
-        <v>37200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>9740457</v>
-      </c>
-      <c r="B51" t="s">
-        <v>177</v>
-      </c>
-      <c r="C51" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" t="s">
-        <v>112</v>
-      </c>
-      <c r="E51" t="s">
-        <v>126</v>
       </c>
       <c r="F51">
         <v>36870</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
+        <v>9728253</v>
+      </c>
+      <c r="B52" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" t="s">
+        <v>125</v>
+      </c>
+      <c r="F52">
+        <v>37200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>9740457</v>
+      </c>
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" t="s">
+        <v>125</v>
+      </c>
+      <c r="F53">
+        <v>36870</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
         <v>9614517</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" t="s">
+        <v>170</v>
+      </c>
+      <c r="F54">
+        <v>13560</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>9619971</v>
+      </c>
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F55">
+        <v>59360</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>9166778</v>
+      </c>
+      <c r="B56" t="s">
         <v>151</v>
       </c>
-      <c r="C52" t="s">
-        <v>50</v>
-      </c>
-      <c r="D52" t="s">
-        <v>112</v>
-      </c>
-      <c r="E52" t="s">
-        <v>171</v>
-      </c>
-      <c r="F52">
-        <v>13560</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>9619971</v>
-      </c>
-      <c r="B53" t="s">
-        <v>148</v>
-      </c>
-      <c r="C53" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" t="s">
-        <v>110</v>
-      </c>
-      <c r="E53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F53">
-        <v>59360</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>9166778</v>
-      </c>
-      <c r="B54" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>52</v>
       </c>
-      <c r="D54" t="s">
-        <v>110</v>
-      </c>
-      <c r="E54" t="s">
-        <v>127</v>
-      </c>
-      <c r="F54">
-        <v>54840</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>9120841</v>
-      </c>
-      <c r="B55" t="s">
-        <v>152</v>
-      </c>
-      <c r="C55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" t="s">
-        <v>110</v>
-      </c>
-      <c r="E55" t="s">
-        <v>127</v>
-      </c>
-      <c r="F55">
-        <v>54840</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>9146467</v>
-      </c>
-      <c r="B56" t="s">
-        <v>152</v>
-      </c>
-      <c r="C56" t="s">
-        <v>172</v>
-      </c>
-      <c r="D56" t="s">
-        <v>110</v>
-      </c>
       <c r="E56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F56">
         <v>54840</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
+        <v>9313967</v>
+      </c>
+      <c r="B57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>8420892</v>
+      </c>
+      <c r="B58" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" t="s">
+        <v>126</v>
+      </c>
+      <c r="F58">
+        <v>54840</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>9219795</v>
+      </c>
+      <c r="B59" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" t="s">
+        <v>179</v>
+      </c>
+      <c r="D59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>9120841</v>
+      </c>
+      <c r="B60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60">
+        <v>54840</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>9166780</v>
+      </c>
+      <c r="B61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>9120853</v>
+      </c>
+      <c r="B62" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" t="s">
+        <v>181</v>
+      </c>
+      <c r="D62" t="s">
+        <v>109</v>
+      </c>
+      <c r="E62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F62">
+        <v>54840</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>9153850</v>
+      </c>
+      <c r="B63" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>9313931</v>
+      </c>
+      <c r="B64" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>9214903</v>
+      </c>
+      <c r="B65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" t="s">
+        <v>184</v>
+      </c>
+      <c r="D65" t="s">
+        <v>109</v>
+      </c>
+      <c r="E65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F65">
+        <v>54840</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
+        <v>9313943</v>
+      </c>
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>9214898</v>
+      </c>
+      <c r="B67" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" t="s">
+        <v>186</v>
+      </c>
+      <c r="D67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E67" t="s">
+        <v>126</v>
+      </c>
+      <c r="F67">
+        <v>54840</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>9120853</v>
+      </c>
+      <c r="B68" t="s">
+        <v>151</v>
+      </c>
+      <c r="C68" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>9146479</v>
+      </c>
+      <c r="B69" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
+        <v>9146467</v>
+      </c>
+      <c r="B70" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
         <v>9662019</v>
       </c>
-      <c r="B57" t="s">
-        <v>142</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" t="s">
         <v>54</v>
       </c>
-      <c r="D57" t="s">
-        <v>110</v>
-      </c>
-      <c r="E57" t="s">
-        <v>114</v>
-      </c>
-      <c r="F57">
+      <c r="D71" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" t="s">
+        <v>113</v>
+      </c>
+      <c r="F71">
         <v>7310</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
         <v>9906049</v>
       </c>
-      <c r="B58" t="s">
-        <v>153</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B72" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72" t="s">
         <v>55</v>
       </c>
-      <c r="D58" t="s">
-        <v>111</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E72" t="s">
+        <v>127</v>
+      </c>
+      <c r="F72">
+        <v>7310</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>9906037</v>
+      </c>
+      <c r="B73" t="s">
+        <v>152</v>
+      </c>
+      <c r="C73" t="s">
+        <v>56</v>
+      </c>
+      <c r="D73" t="s">
+        <v>110</v>
+      </c>
+      <c r="E73" t="s">
+        <v>127</v>
+      </c>
+      <c r="F73">
+        <v>15750</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>9906025</v>
+      </c>
+      <c r="B74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" t="s">
+        <v>110</v>
+      </c>
+      <c r="E74" t="s">
+        <v>127</v>
+      </c>
+      <c r="F74">
+        <v>23542</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>9906013</v>
+      </c>
+      <c r="B75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E75" t="s">
+        <v>127</v>
+      </c>
+      <c r="F75">
+        <v>15742</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
+        <v>9966233</v>
+      </c>
+      <c r="B76" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E76" t="s">
         <v>128</v>
       </c>
-      <c r="F58">
-        <v>7310</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>9906037</v>
-      </c>
-      <c r="B59" t="s">
-        <v>153</v>
-      </c>
-      <c r="C59" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" t="s">
-        <v>111</v>
-      </c>
-      <c r="E59" t="s">
-        <v>128</v>
-      </c>
-      <c r="F59">
-        <v>15750</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>9906025</v>
-      </c>
-      <c r="B60" t="s">
-        <v>153</v>
-      </c>
-      <c r="C60" t="s">
-        <v>57</v>
-      </c>
-      <c r="D60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" t="s">
-        <v>128</v>
-      </c>
-      <c r="F60">
-        <v>23542</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>9906013</v>
-      </c>
-      <c r="B61" t="s">
-        <v>153</v>
-      </c>
-      <c r="C61" t="s">
-        <v>58</v>
-      </c>
-      <c r="D61" t="s">
-        <v>111</v>
-      </c>
-      <c r="E61" t="s">
-        <v>128</v>
-      </c>
-      <c r="F61">
-        <v>15742</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>9966233</v>
-      </c>
-      <c r="B62" t="s">
-        <v>153</v>
-      </c>
-      <c r="C62" t="s">
-        <v>59</v>
-      </c>
-      <c r="D62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="F76">
+        <v>11400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
+        <v>9745524</v>
+      </c>
+      <c r="B77" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" t="s">
+        <v>110</v>
+      </c>
+      <c r="E77" t="s">
+        <v>163</v>
+      </c>
+      <c r="F77">
+        <v>9960</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
+        <v>9315446</v>
+      </c>
+      <c r="B78" t="s">
+        <v>145</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
+        <v>109</v>
+      </c>
+      <c r="E78" t="s">
         <v>129</v>
       </c>
-      <c r="F62">
-        <v>11400</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>9745524</v>
-      </c>
-      <c r="B63" t="s">
-        <v>142</v>
-      </c>
-      <c r="C63" t="s">
-        <v>60</v>
-      </c>
-      <c r="D63" t="s">
-        <v>111</v>
-      </c>
-      <c r="E63" t="s">
-        <v>164</v>
-      </c>
-      <c r="F63">
-        <v>9960</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>9315446</v>
-      </c>
-      <c r="B64" t="s">
-        <v>146</v>
-      </c>
-      <c r="C64" t="s">
-        <v>61</v>
-      </c>
-      <c r="D64" t="s">
-        <v>110</v>
-      </c>
-      <c r="E64" t="s">
-        <v>130</v>
-      </c>
-      <c r="F64">
+      <c r="F78">
         <v>15540</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
         <v>9401790</v>
       </c>
-      <c r="B65" t="s">
-        <v>146</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" t="s">
         <v>62</v>
-      </c>
-      <c r="D65" t="s">
-        <v>112</v>
-      </c>
-      <c r="E65" t="s">
-        <v>131</v>
-      </c>
-      <c r="F65">
-        <v>12268</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>9319674</v>
-      </c>
-      <c r="B66" t="s">
-        <v>146</v>
-      </c>
-      <c r="C66" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" t="s">
-        <v>112</v>
-      </c>
-      <c r="E66" t="s">
-        <v>131</v>
-      </c>
-      <c r="F66">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>9306639</v>
-      </c>
-      <c r="B67" t="s">
-        <v>146</v>
-      </c>
-      <c r="C67" t="s">
-        <v>64</v>
-      </c>
-      <c r="D67" t="s">
-        <v>113</v>
-      </c>
-      <c r="E67" t="s">
-        <v>132</v>
-      </c>
-      <c r="F67">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>9283291</v>
-      </c>
-      <c r="B68" t="s">
-        <v>146</v>
-      </c>
-      <c r="C68" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" t="s">
-        <v>112</v>
-      </c>
-      <c r="E68" t="s">
-        <v>130</v>
-      </c>
-      <c r="F68">
-        <v>15540</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>9319703</v>
-      </c>
-      <c r="B69" t="s">
-        <v>146</v>
-      </c>
-      <c r="C69" t="s">
-        <v>66</v>
-      </c>
-      <c r="D69" t="s">
-        <v>113</v>
-      </c>
-      <c r="E69" t="s">
-        <v>131</v>
-      </c>
-      <c r="F69">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>9308948</v>
-      </c>
-      <c r="B70" t="s">
-        <v>146</v>
-      </c>
-      <c r="C70" t="s">
-        <v>67</v>
-      </c>
-      <c r="D70" t="s">
-        <v>112</v>
-      </c>
-      <c r="E70" t="s">
-        <v>130</v>
-      </c>
-      <c r="F70">
-        <v>15540</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>9308950</v>
-      </c>
-      <c r="B71" t="s">
-        <v>146</v>
-      </c>
-      <c r="C71" t="s">
-        <v>68</v>
-      </c>
-      <c r="D71" t="s">
-        <v>112</v>
-      </c>
-      <c r="E71" t="s">
-        <v>131</v>
-      </c>
-      <c r="F71">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>9283289</v>
-      </c>
-      <c r="B72" t="s">
-        <v>146</v>
-      </c>
-      <c r="C72" t="s">
-        <v>69</v>
-      </c>
-      <c r="D72" t="s">
-        <v>112</v>
-      </c>
-      <c r="E72" t="s">
-        <v>130</v>
-      </c>
-      <c r="F72">
-        <v>15540</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>9315458</v>
-      </c>
-      <c r="B73" t="s">
-        <v>146</v>
-      </c>
-      <c r="C73" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" t="s">
-        <v>112</v>
-      </c>
-      <c r="E73" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73">
-        <v>15260</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>9598218</v>
-      </c>
-      <c r="B74" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" t="s">
-        <v>71</v>
-      </c>
-      <c r="D74" t="s">
-        <v>112</v>
-      </c>
-      <c r="E74" t="s">
-        <v>167</v>
-      </c>
-      <c r="F74">
-        <v>9760</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>9609146</v>
-      </c>
-      <c r="B75" t="s">
-        <v>147</v>
-      </c>
-      <c r="C75" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" t="s">
-        <v>111</v>
-      </c>
-      <c r="E75" t="s">
-        <v>168</v>
-      </c>
-      <c r="F75">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>9293583</v>
-      </c>
-      <c r="B76" t="s">
-        <v>147</v>
-      </c>
-      <c r="C76" t="s">
-        <v>73</v>
-      </c>
-      <c r="D76" t="s">
-        <v>156</v>
-      </c>
-      <c r="E76" t="s">
-        <v>133</v>
-      </c>
-      <c r="F76">
-        <v>15130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>9293909</v>
-      </c>
-      <c r="B77" t="s">
-        <v>147</v>
-      </c>
-      <c r="C77" t="s">
-        <v>74</v>
-      </c>
-      <c r="D77" t="s">
-        <v>156</v>
-      </c>
-      <c r="E77" t="s">
-        <v>133</v>
-      </c>
-      <c r="F77">
-        <v>15090</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>9542984</v>
-      </c>
-      <c r="B78" t="s">
-        <v>154</v>
-      </c>
-      <c r="C78" t="s">
-        <v>75</v>
-      </c>
-      <c r="D78" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" t="s">
-        <v>134</v>
-      </c>
-      <c r="F78">
-        <v>6100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>9551777</v>
-      </c>
-      <c r="B79" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" t="s">
-        <v>76</v>
       </c>
       <c r="D79" t="s">
         <v>111</v>
       </c>
       <c r="E79" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F79">
-        <v>5800</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12268</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
-        <v>9702209</v>
+        <v>9319674</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C80" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D80" t="s">
         <v>111</v>
       </c>
       <c r="E80" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F80">
-        <v>7180</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
-        <v>9702194</v>
+        <v>9306639</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C81" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D81" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E81" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F81">
-        <v>7180</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
-        <v>9702211</v>
+        <v>9283291</v>
       </c>
       <c r="B82" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C82" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D82" t="s">
         <v>111</v>
       </c>
       <c r="E82" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F82">
-        <v>7180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
-        <v>9849992</v>
+        <v>9319703</v>
       </c>
       <c r="B83" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C83" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D83" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E83" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F83">
-        <v>10850</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
-        <v>9850006</v>
+        <v>9308948</v>
       </c>
       <c r="B84" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C84" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
       </c>
       <c r="E84" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F84">
-        <v>10850</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
-        <v>9712864</v>
+        <v>9308950</v>
       </c>
       <c r="B85" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C85" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D85" t="s">
         <v>111</v>
       </c>
       <c r="E85" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F85">
-        <v>14280</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
-        <v>9904871</v>
+        <v>9283289</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C86" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="D86" t="s">
+        <v>111</v>
+      </c>
+      <c r="E86" t="s">
+        <v>129</v>
+      </c>
+      <c r="F86">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
-        <v>9798002</v>
+        <v>9315458</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C87" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D87" t="s">
         <v>111</v>
       </c>
       <c r="E87" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F87">
-        <v>11494</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15260</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
-        <v>9797981</v>
+        <v>9598218</v>
       </c>
       <c r="B88" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C88" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D88" t="s">
         <v>111</v>
       </c>
       <c r="E88" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F88">
+        <v>9760</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
+        <v>9609146</v>
+      </c>
+      <c r="B89" t="s">
+        <v>146</v>
+      </c>
+      <c r="C89" t="s">
+        <v>72</v>
+      </c>
+      <c r="D89" t="s">
+        <v>110</v>
+      </c>
+      <c r="E89" t="s">
+        <v>167</v>
+      </c>
+      <c r="F89">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
+        <v>9293583</v>
+      </c>
+      <c r="B90" t="s">
+        <v>146</v>
+      </c>
+      <c r="C90" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" t="s">
+        <v>155</v>
+      </c>
+      <c r="E90" t="s">
+        <v>132</v>
+      </c>
+      <c r="F90">
+        <v>15130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
+        <v>9293909</v>
+      </c>
+      <c r="B91" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" t="s">
+        <v>74</v>
+      </c>
+      <c r="D91" t="s">
+        <v>155</v>
+      </c>
+      <c r="E91" t="s">
+        <v>132</v>
+      </c>
+      <c r="F91">
+        <v>15090</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>9542984</v>
+      </c>
+      <c r="B92" t="s">
+        <v>153</v>
+      </c>
+      <c r="C92" t="s">
+        <v>75</v>
+      </c>
+      <c r="D92" t="s">
+        <v>110</v>
+      </c>
+      <c r="E92" t="s">
+        <v>133</v>
+      </c>
+      <c r="F92">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>9551777</v>
+      </c>
+      <c r="B93" t="s">
+        <v>153</v>
+      </c>
+      <c r="C93" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" t="s">
+        <v>110</v>
+      </c>
+      <c r="E93" t="s">
+        <v>134</v>
+      </c>
+      <c r="F93">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>9702209</v>
+      </c>
+      <c r="B94" t="s">
+        <v>154</v>
+      </c>
+      <c r="C94" t="s">
+        <v>77</v>
+      </c>
+      <c r="D94" t="s">
+        <v>110</v>
+      </c>
+      <c r="E94" t="s">
+        <v>135</v>
+      </c>
+      <c r="F94">
+        <v>7180</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
+        <v>9702194</v>
+      </c>
+      <c r="B95" t="s">
+        <v>154</v>
+      </c>
+      <c r="C95" t="s">
+        <v>78</v>
+      </c>
+      <c r="D95" t="s">
+        <v>110</v>
+      </c>
+      <c r="E95" t="s">
+        <v>135</v>
+      </c>
+      <c r="F95">
+        <v>7180</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
+        <v>9702211</v>
+      </c>
+      <c r="B96" t="s">
+        <v>154</v>
+      </c>
+      <c r="C96" t="s">
+        <v>79</v>
+      </c>
+      <c r="D96" t="s">
+        <v>110</v>
+      </c>
+      <c r="E96" t="s">
+        <v>135</v>
+      </c>
+      <c r="F96">
+        <v>7180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
+        <v>9849992</v>
+      </c>
+      <c r="B97" t="s">
+        <v>154</v>
+      </c>
+      <c r="C97" t="s">
+        <v>80</v>
+      </c>
+      <c r="D97" t="s">
+        <v>110</v>
+      </c>
+      <c r="E97" t="s">
+        <v>135</v>
+      </c>
+      <c r="F97">
+        <v>10850</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>9850006</v>
+      </c>
+      <c r="B98" t="s">
+        <v>154</v>
+      </c>
+      <c r="C98" t="s">
+        <v>81</v>
+      </c>
+      <c r="D98" t="s">
+        <v>110</v>
+      </c>
+      <c r="E98" t="s">
+        <v>135</v>
+      </c>
+      <c r="F98">
+        <v>10850</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>9712864</v>
+      </c>
+      <c r="B99" t="s">
+        <v>154</v>
+      </c>
+      <c r="C99" t="s">
+        <v>82</v>
+      </c>
+      <c r="D99" t="s">
+        <v>110</v>
+      </c>
+      <c r="E99" t="s">
+        <v>136</v>
+      </c>
+      <c r="F99">
+        <v>14280</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>9904871</v>
+      </c>
+      <c r="B100" t="s">
+        <v>154</v>
+      </c>
+      <c r="C100" t="s">
+        <v>83</v>
+      </c>
+      <c r="D100" t="s">
+        <v>110</v>
+      </c>
+      <c r="E100" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
+        <v>9798002</v>
+      </c>
+      <c r="B101" t="s">
+        <v>154</v>
+      </c>
+      <c r="C101" t="s">
+        <v>84</v>
+      </c>
+      <c r="D101" t="s">
+        <v>110</v>
+      </c>
+      <c r="E101" t="s">
+        <v>136</v>
+      </c>
+      <c r="F101">
         <v>11494</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <v>9797993</v>
-      </c>
-      <c r="B89" t="s">
-        <v>155</v>
-      </c>
-      <c r="C89" t="s">
-        <v>86</v>
-      </c>
-      <c r="D89" t="s">
-        <v>111</v>
-      </c>
-      <c r="E89" t="s">
-        <v>137</v>
-      </c>
-      <c r="F89">
-        <v>11494</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>9798014</v>
-      </c>
-      <c r="B90" t="s">
-        <v>155</v>
-      </c>
-      <c r="C90" t="s">
-        <v>87</v>
-      </c>
-      <c r="D90" t="s">
-        <v>111</v>
-      </c>
-      <c r="E90" t="s">
-        <v>137</v>
-      </c>
-      <c r="F90">
-        <v>11494</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>9904883</v>
-      </c>
-      <c r="B91" t="s">
-        <v>155</v>
-      </c>
-      <c r="C91" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>9701554</v>
-      </c>
-      <c r="B92" t="s">
-        <v>155</v>
-      </c>
-      <c r="C92" t="s">
-        <v>89</v>
-      </c>
-      <c r="D92" t="s">
-        <v>112</v>
-      </c>
-      <c r="E92" t="s">
-        <v>117</v>
-      </c>
-      <c r="F92">
-        <v>18035</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>9701566</v>
-      </c>
-      <c r="B93" t="s">
-        <v>155</v>
-      </c>
-      <c r="C93" t="s">
-        <v>90</v>
-      </c>
-      <c r="D93" t="s">
-        <v>112</v>
-      </c>
-      <c r="E93" t="s">
-        <v>117</v>
-      </c>
-      <c r="F93">
-        <v>18035</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A94">
-        <v>9694646</v>
-      </c>
-      <c r="B94" t="s">
-        <v>155</v>
-      </c>
-      <c r="C94" t="s">
-        <v>91</v>
-      </c>
-      <c r="D94" t="s">
-        <v>112</v>
-      </c>
-      <c r="E94" t="s">
-        <v>117</v>
-      </c>
-      <c r="F94">
-        <v>18035</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>9375616</v>
-      </c>
-      <c r="B95" t="s">
-        <v>155</v>
-      </c>
-      <c r="C95" t="s">
-        <v>92</v>
-      </c>
-      <c r="D95" t="s">
-        <v>112</v>
-      </c>
-      <c r="E95" t="s">
-        <v>138</v>
-      </c>
-      <c r="F95">
-        <v>11340</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>9390769</v>
-      </c>
-      <c r="B96" t="s">
-        <v>155</v>
-      </c>
-      <c r="C96" t="s">
-        <v>93</v>
-      </c>
-      <c r="D96" t="s">
-        <v>112</v>
-      </c>
-      <c r="E96" t="s">
-        <v>138</v>
-      </c>
-      <c r="F96">
-        <v>11636</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>9392470</v>
-      </c>
-      <c r="B97" t="s">
-        <v>155</v>
-      </c>
-      <c r="C97" t="s">
-        <v>94</v>
-      </c>
-      <c r="D97" t="s">
-        <v>112</v>
-      </c>
-      <c r="E97" t="s">
-        <v>138</v>
-      </c>
-      <c r="F97">
-        <v>11620</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>9392468</v>
-      </c>
-      <c r="B98" t="s">
-        <v>155</v>
-      </c>
-      <c r="C98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D98" t="s">
-        <v>112</v>
-      </c>
-      <c r="E98" t="s">
-        <v>138</v>
-      </c>
-      <c r="F98">
-        <v>11620</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>9392482</v>
-      </c>
-      <c r="B99" t="s">
-        <v>155</v>
-      </c>
-      <c r="C99" t="s">
-        <v>96</v>
-      </c>
-      <c r="D99" t="s">
-        <v>112</v>
-      </c>
-      <c r="E99" t="s">
-        <v>138</v>
-      </c>
-      <c r="F99">
-        <v>11620</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A100">
-        <v>9836050</v>
-      </c>
-      <c r="B100" t="s">
-        <v>155</v>
-      </c>
-      <c r="C100" t="s">
-        <v>97</v>
-      </c>
-      <c r="D100" t="s">
-        <v>111</v>
-      </c>
-      <c r="E100" t="s">
-        <v>136</v>
-      </c>
-      <c r="F100">
-        <v>10320</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A101">
-        <v>9797723</v>
-      </c>
-      <c r="B101" t="s">
-        <v>155</v>
-      </c>
-      <c r="C101" t="s">
-        <v>98</v>
-      </c>
-      <c r="D101" t="s">
-        <v>111</v>
-      </c>
-      <c r="E101" t="s">
-        <v>139</v>
-      </c>
-      <c r="F101">
-        <v>7180</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
-        <v>9854791</v>
+        <v>9797981</v>
       </c>
       <c r="B102" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C102" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D102" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E102" t="s">
         <v>136</v>
       </c>
       <c r="F102">
-        <v>10320</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11494</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
-        <v>9854806</v>
+        <v>9797993</v>
       </c>
       <c r="B103" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C103" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="D103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E103" t="s">
         <v>136</v>
       </c>
       <c r="F103">
-        <v>10320</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11494</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
-        <v>9836036</v>
+        <v>9798014</v>
       </c>
       <c r="B104" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C104" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D104" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E104" t="s">
         <v>136</v>
       </c>
       <c r="F104">
-        <v>10320</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11494</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
-        <v>9836062</v>
+        <v>9904883</v>
       </c>
       <c r="B105" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C105" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D105" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E105" t="s">
-        <v>136</v>
-      </c>
-      <c r="F105">
-        <v>10320</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A106">
-        <v>9854789</v>
+        <v>9701554</v>
       </c>
       <c r="B106" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C106" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D106" t="s">
         <v>111</v>
       </c>
       <c r="E106" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="F106">
-        <v>10320</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+        <v>18035</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A107">
-        <v>9836048</v>
+        <v>9701566</v>
       </c>
       <c r="B107" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C107" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D107" t="s">
         <v>111</v>
       </c>
       <c r="E107" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="F107">
-        <v>10320</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+        <v>18035</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A108">
-        <v>9797735</v>
+        <v>9694646</v>
       </c>
       <c r="B108" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C108" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="D108" t="s">
         <v>111</v>
       </c>
       <c r="E108" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="F108">
-        <v>7180</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+        <v>18035</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A109">
-        <v>9712319</v>
+        <v>9375616</v>
       </c>
       <c r="B109" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C109" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
       </c>
       <c r="E109" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F109">
-        <v>7317</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
-        <v>9712321</v>
+        <v>9390769</v>
       </c>
       <c r="B110" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C110" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D110" t="s">
         <v>111</v>
       </c>
       <c r="E110" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F110">
-        <v>7317</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11636</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A111">
-        <v>9726475</v>
+        <v>9392470</v>
       </c>
       <c r="B111" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C111" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D111" t="s">
         <v>111</v>
       </c>
       <c r="E111" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F111">
-        <v>7317</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11620</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A112">
-        <v>9775737</v>
+        <v>9392468</v>
       </c>
       <c r="B112" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C112" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D112" t="s">
         <v>111</v>
       </c>
       <c r="E112" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="F112">
+        <v>11620</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113">
+        <v>9392482</v>
+      </c>
+      <c r="B113" t="s">
+        <v>154</v>
+      </c>
+      <c r="C113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D113" t="s">
+        <v>111</v>
+      </c>
+      <c r="E113" t="s">
+        <v>137</v>
+      </c>
+      <c r="F113">
+        <v>11620</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114">
+        <v>9836050</v>
+      </c>
+      <c r="B114" t="s">
+        <v>154</v>
+      </c>
+      <c r="C114" t="s">
+        <v>97</v>
+      </c>
+      <c r="D114" t="s">
+        <v>110</v>
+      </c>
+      <c r="E114" t="s">
+        <v>135</v>
+      </c>
+      <c r="F114">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115">
+        <v>9797723</v>
+      </c>
+      <c r="B115" t="s">
+        <v>154</v>
+      </c>
+      <c r="C115" t="s">
+        <v>98</v>
+      </c>
+      <c r="D115" t="s">
+        <v>110</v>
+      </c>
+      <c r="E115" t="s">
+        <v>138</v>
+      </c>
+      <c r="F115">
+        <v>7180</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116">
+        <v>9854791</v>
+      </c>
+      <c r="B116" t="s">
+        <v>154</v>
+      </c>
+      <c r="C116" t="s">
+        <v>99</v>
+      </c>
+      <c r="D116" t="s">
+        <v>110</v>
+      </c>
+      <c r="E116" t="s">
+        <v>135</v>
+      </c>
+      <c r="F116">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117">
+        <v>9854806</v>
+      </c>
+      <c r="B117" t="s">
+        <v>154</v>
+      </c>
+      <c r="C117" t="s">
+        <v>100</v>
+      </c>
+      <c r="D117" t="s">
+        <v>110</v>
+      </c>
+      <c r="E117" t="s">
+        <v>135</v>
+      </c>
+      <c r="F117">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118">
+        <v>9836036</v>
+      </c>
+      <c r="B118" t="s">
+        <v>154</v>
+      </c>
+      <c r="C118" t="s">
+        <v>101</v>
+      </c>
+      <c r="D118" t="s">
+        <v>110</v>
+      </c>
+      <c r="E118" t="s">
+        <v>135</v>
+      </c>
+      <c r="F118">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119">
+        <v>9836062</v>
+      </c>
+      <c r="B119" t="s">
+        <v>154</v>
+      </c>
+      <c r="C119" t="s">
+        <v>102</v>
+      </c>
+      <c r="D119" t="s">
+        <v>110</v>
+      </c>
+      <c r="E119" t="s">
+        <v>135</v>
+      </c>
+      <c r="F119">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120">
+        <v>9854789</v>
+      </c>
+      <c r="B120" t="s">
+        <v>154</v>
+      </c>
+      <c r="C120" t="s">
+        <v>103</v>
+      </c>
+      <c r="D120" t="s">
+        <v>110</v>
+      </c>
+      <c r="E120" t="s">
+        <v>135</v>
+      </c>
+      <c r="F120">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121">
+        <v>9836048</v>
+      </c>
+      <c r="B121" t="s">
+        <v>154</v>
+      </c>
+      <c r="C121" t="s">
+        <v>104</v>
+      </c>
+      <c r="D121" t="s">
+        <v>110</v>
+      </c>
+      <c r="E121" t="s">
+        <v>135</v>
+      </c>
+      <c r="F121">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122">
+        <v>9797735</v>
+      </c>
+      <c r="B122" t="s">
+        <v>154</v>
+      </c>
+      <c r="C122" t="s">
+        <v>105</v>
+      </c>
+      <c r="D122" t="s">
+        <v>110</v>
+      </c>
+      <c r="E122" t="s">
+        <v>138</v>
+      </c>
+      <c r="F122">
+        <v>7180</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123">
+        <v>9712319</v>
+      </c>
+      <c r="B123" t="s">
+        <v>154</v>
+      </c>
+      <c r="C123" t="s">
+        <v>106</v>
+      </c>
+      <c r="D123" t="s">
+        <v>110</v>
+      </c>
+      <c r="E123" t="s">
+        <v>138</v>
+      </c>
+      <c r="F123">
+        <v>7317</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124">
+        <v>9712321</v>
+      </c>
+      <c r="B124" t="s">
+        <v>154</v>
+      </c>
+      <c r="C124" t="s">
+        <v>107</v>
+      </c>
+      <c r="D124" t="s">
+        <v>110</v>
+      </c>
+      <c r="E124" t="s">
+        <v>138</v>
+      </c>
+      <c r="F124">
+        <v>7317</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125">
+        <v>9726475</v>
+      </c>
+      <c r="B125" t="s">
+        <v>154</v>
+      </c>
+      <c r="C125" t="s">
+        <v>190</v>
+      </c>
+      <c r="D125" t="s">
+        <v>110</v>
+      </c>
+      <c r="E125" t="s">
+        <v>138</v>
+      </c>
+      <c r="F125">
+        <v>7317</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126">
+        <v>9775737</v>
+      </c>
+      <c r="B126" t="s">
+        <v>147</v>
+      </c>
+      <c r="C126" t="s">
+        <v>108</v>
+      </c>
+      <c r="D126" t="s">
+        <v>110</v>
+      </c>
+      <c r="E126" t="s">
+        <v>114</v>
+      </c>
+      <c r="F126">
         <v>17279</v>
       </c>
     </row>
@@ -3172,8 +3447,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000B73ECAA2334A14EB365ED6608A878E1" ma:contentTypeVersion="20" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="3a0a8eb6936e710403338e49b0d9cf8c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6e040d9b-4d00-4c60-b912-ca778ccae294" xmlns:ns3="e92f16c9-db69-4522-84e2-bf933696a321" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="879cce07b0e372e82448d845ce3e64df" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000B73ECAA2334A14EB365ED6608A878E1" ma:contentTypeVersion="20" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="aa261c57a18327ad4c092a13a9f1b96d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6e040d9b-4d00-4c60-b912-ca778ccae294" xmlns:ns3="e92f16c9-db69-4522-84e2-bf933696a321" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ada142b233870dd5f0255efd6e0c4bae" ns2:_="" ns3:_="">
     <xsd:import namespace="6e040d9b-4d00-4c60-b912-ca778ccae294"/>
     <xsd:import namespace="e92f16c9-db69-4522-84e2-bf933696a321"/>
     <xsd:element name="properties">
@@ -3438,15 +3722,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABB72383-3208-4DA4-A3CB-6496336595CC}">
   <ds:schemaRefs>
@@ -3459,28 +3734,13 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3719BABF-6018-4300-8EF8-A21D23A9485A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{855F6443-400B-4276-AA3F-D8A900D50BF5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6e040d9b-4d00-4c60-b912-ca778ccae294"/>
-    <ds:schemaRef ds:uri="e92f16c9-db69-4522-84e2-bf933696a321"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{855F6443-400B-4276-AA3F-D8A900D50BF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3BECD9-BD61-4DD0-AD49-ADAA4A55C970}"/>
 </file>
</xml_diff>